<commit_message>
1st phase of development is done
</commit_message>
<xml_diff>
--- a/Data/Input/Input.xlsx
+++ b/Data/Input/Input.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f8b04ab2bc622ed/Documents/git/NaukriProcess/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="74" documentId="11_F25DC773A252ABDACC10488E315C47985BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7BE371BE-11BB-4FAA-A570-A466AE6ED3E4}"/>
+  <xr:revisionPtr revIDLastSave="89" documentId="11_F25DC773A252ABDACC10488E315C47985BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BE81147-39B9-405D-AE76-23E15DC25C94}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="29">
   <si>
     <t>Name</t>
   </si>
@@ -94,16 +94,25 @@
     <t>15 years</t>
   </si>
   <si>
-    <t>Chethan</t>
-  </si>
-  <si>
-    <t>chethan.rpa@gmail.com</t>
-  </si>
-  <si>
-    <t>UiPath, RPA, Power Automate</t>
-  </si>
-  <si>
-    <t>Hyderabad,Bangalore,Chennai</t>
+    <t>Sriharshini</t>
+  </si>
+  <si>
+    <t>peddisriharshini@gmail.com</t>
+  </si>
+  <si>
+    <t>Hyderabad,Bangalore</t>
+  </si>
+  <si>
+    <t>chandrikagollashetti@gmail.com</t>
+  </si>
+  <si>
+    <t>Chandrika</t>
+  </si>
+  <si>
+    <t>Fresher,Software Engineer, Software Developer, Software Tester, UiPath</t>
+  </si>
+  <si>
+    <t>Fresher,Software Engineer, Software Developer, Software Tester</t>
   </si>
 </sst>
 </file>
@@ -474,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -511,17 +520,34 @@
       <c r="A2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>23</v>
       </c>
       <c r="C2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="5" t="s">
         <v>25</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed the process for Email
</commit_message>
<xml_diff>
--- a/Data/Input/Input.xlsx
+++ b/Data/Input/Input.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/5f8b04ab2bc622ed/Documents/git/NaukriProcess/Data/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="89" documentId="11_F25DC773A252ABDACC10488E315C47985BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BE81147-39B9-405D-AE76-23E15DC25C94}"/>
+  <xr:revisionPtr revIDLastSave="90" documentId="11_F25DC773A252ABDACC10488E315C47985BDE58EE" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DEB93DE4-E89F-4639-AC05-9583544FC9D6}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -486,7 +486,7 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -544,7 +544,7 @@
         <v>28</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E3" s="5" t="s">
         <v>24</v>

</xml_diff>